<commit_message>
Update DateBase/orders/International Ever Green_2025-10-15.xlsx
</commit_message>
<xml_diff>
--- a/DateBase/orders/International Ever Green_2025-10-15.xlsx
+++ b/DateBase/orders/International Ever Green_2025-10-15.xlsx
@@ -528,6 +528,9 @@
       <c r="C11" t="str">
         <v>454_蓝星花_tweedia blue_undefined_1bunch</v>
       </c>
+      <c r="F11" t="str">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
@@ -589,7 +592,7 @@
         <v>0.00</v>
       </c>
       <c r="G2" t="str">
-        <v>015205205803030200</v>
+        <v>015205205803030205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>